<commit_message>
pequeña corrección en la escaleta LE_06_06_CO
Se introdujo un cambio en las observaciones
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/ESCALETA_LE_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/ESCALETA_LE_06_06_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="311">
   <si>
     <t>Asignatura</t>
   </si>
@@ -934,9 +934,6 @@
     <t>DBA2. Realizar un recurso que motive a los estudiantes a escribir poemas mediante diversos ejercicios de sensibilización a la poesía. Se pueden plantear ejercicios sobre los sentidos o sobre los sentimientos relacioandos con la creación de versos</t>
   </si>
   <si>
-    <t>DBA6. Buscar un editorial. Lo podemos convertir en pdf e imagen y luego usarlo para aplicarle etiquetas con sus principales partes.</t>
-  </si>
-  <si>
     <t>DBA6. Revisar que el lenguaje se adapte al contexto colombiano y cambiar todo lo que haga referencia a "artículo" por "columna"</t>
   </si>
   <si>
@@ -980,6 +977,9 @@
   </si>
   <si>
     <t>DBA10. Hacer contenedores para el editorial, la columna de opinión y el debate, incluyendo sus principales características (la idea es mostrar las diferencias entre ellos).</t>
+  </si>
+  <si>
+    <t>DBA6. Buscar un editorial. Lo podemos convertir en pdf e imagen y luego usarlo para aplicarle etiquetas con sus principales partes. Aprovechar lo hecho anteriormente en LE_06_11_REC30</t>
   </si>
 </sst>
 </file>
@@ -1260,34 +1260,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1327,6 +1309,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1635,9 +1635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
+      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,94 +1665,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="33" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="48"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2028,7 +2028,7 @@
         <v>36</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -2065,7 +2065,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -2144,7 +2144,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>19</v>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -2506,7 +2506,7 @@
         <v>36</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>20</v>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2622,7 +2622,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2740,7 +2740,7 @@
         <v>24</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2798,10 +2798,10 @@
       </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="O20" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>307</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>19</v>
@@ -3039,7 +3039,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>19</v>
@@ -3159,7 +3159,7 @@
         <v>41</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>19</v>
@@ -3218,7 +3218,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>19</v>
@@ -3277,7 +3277,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>19</v>
@@ -3698,7 +3698,7 @@
         <v>43</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>19</v>
@@ -3816,7 +3816,7 @@
         <v>43</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P37" s="9" t="s">
         <v>19</v>
@@ -5280,6 +5280,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5294,12 +5300,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
LE: Esqueletos 0606, 0607, 0608, 0707, 0708
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/ESCALETA_LE_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/ESCALETA_LE_06_06_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\CRISTIAN\PLANETA\NUEVO\ESCALETAS\Escaletas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado06\guion06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="311">
   <si>
     <t>Asignatura</t>
   </si>
@@ -426,9 +426,6 @@
   </si>
   <si>
     <t>Recurso M102AB-01</t>
-  </si>
-  <si>
-    <t>LE_06_06_C0</t>
   </si>
   <si>
     <t>Lectura: las composiciones de arte menor y de arte mayor</t>
@@ -980,6 +977,9 @@
   </si>
   <si>
     <t>DBA6. Buscar un editorial. Lo podemos convertir en pdf e imagen y luego usarlo para aplicarle etiquetas con sus principales partes. Aprovechar lo hecho anteriormente en LE_06_11_REC30</t>
+  </si>
+  <si>
+    <t>LE_06_06_CO</t>
   </si>
 </sst>
 </file>
@@ -1260,16 +1260,34 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1309,24 +1327,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1635,142 +1635,142 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="54.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="72.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="72.59765625" customWidth="1"/>
+    <col min="11" max="11" width="13.265625" customWidth="1"/>
+    <col min="12" max="12" width="17.3984375" customWidth="1"/>
+    <col min="13" max="14" width="9.265625" customWidth="1"/>
+    <col min="15" max="15" width="255.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.59765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.3984375" style="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="42"/>
+    <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="51"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.25" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1779,7 +1779,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1792,7 +1792,7 @@
         <v>43</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P3" s="21" t="s">
         <v>19</v>
@@ -1807,29 +1807,29 @@
         <v>130</v>
       </c>
       <c r="T3" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U3" s="22" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1838,7 +1838,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1851,7 +1851,7 @@
         <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1866,29 +1866,29 @@
         <v>130</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U4" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1897,7 +1897,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1910,7 +1910,7 @@
         <v>24</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1925,29 +1925,29 @@
         <v>130</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U5" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1956,7 +1956,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1969,7 +1969,7 @@
         <v>48</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1984,29 +1984,29 @@
         <v>130</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U6" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -2015,7 +2015,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -2028,7 +2028,7 @@
         <v>36</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -2043,29 +2043,29 @@
         <v>130</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U7" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -2074,7 +2074,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -2087,7 +2087,7 @@
         <v>29</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -2102,29 +2102,29 @@
         <v>130</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U8" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C9" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -2133,7 +2133,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -2144,7 +2144,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>19</v>
@@ -2153,35 +2153,35 @@
         <v>7</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S9" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="T9" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="U9" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="U9" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -2190,7 +2190,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -2212,37 +2212,37 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="S10" s="10" t="s">
+      <c r="T10" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="T10" s="12" t="s">
+      <c r="U10" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="U10" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C11" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -2251,7 +2251,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2262,46 +2262,46 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S11" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="S11" s="10" t="s">
+      <c r="T11" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="T11" s="12" t="s">
+      <c r="U11" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="U11" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C12" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>137</v>
-      </c>
       <c r="E12" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -2310,7 +2310,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2323,7 +2323,7 @@
         <v>27</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -2338,31 +2338,31 @@
         <v>130</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C13" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>137</v>
-      </c>
       <c r="E13" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2371,7 +2371,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2384,7 +2384,7 @@
         <v>23</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2399,31 +2399,31 @@
         <v>130</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C14" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2432,7 +2432,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2445,7 +2445,7 @@
         <v>121</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>19</v>
@@ -2460,31 +2460,31 @@
         <v>130</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C15" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2493,7 +2493,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2506,7 +2506,7 @@
         <v>36</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>20</v>
@@ -2521,29 +2521,29 @@
         <v>130</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2552,7 +2552,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2574,35 +2574,35 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="S16" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>206</v>
-      </c>
       <c r="T16" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H17" s="9">
         <v>15</v>
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>19</v>
@@ -2622,44 +2622,44 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S17" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="T17" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="T17" s="12" t="s">
+      <c r="U17" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="U17" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2668,7 +2668,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>19</v>
@@ -2679,7 +2679,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2688,37 +2688,37 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S18" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="S18" s="10" t="s">
+      <c r="T18" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="U18" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="T18" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="U18" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2727,7 +2727,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2740,7 +2740,7 @@
         <v>24</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2755,31 +2755,31 @@
         <v>130</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2788,7 +2788,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2798,10 +2798,10 @@
       </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="O20" s="9" t="s">
         <v>305</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>306</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>19</v>
@@ -2816,29 +2816,29 @@
         <v>130</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2847,7 +2847,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>19</v>
@@ -2869,37 +2869,37 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="S21" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>206</v>
-      </c>
       <c r="T21" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2908,7 +2908,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2921,7 +2921,7 @@
         <v>45</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>19</v>
@@ -2936,31 +2936,31 @@
         <v>130</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>123</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
@@ -2969,7 +2969,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2982,7 +2982,7 @@
         <v>121</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>19</v>
@@ -2997,29 +2997,29 @@
         <v>130</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -3028,7 +3028,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>19</v>
@@ -3039,7 +3039,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>19</v>
@@ -3048,35 +3048,35 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
@@ -3085,7 +3085,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -3098,7 +3098,7 @@
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -3107,37 +3107,37 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="S25" s="10" t="s">
-        <v>206</v>
-      </c>
       <c r="T25" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>144</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" s="9">
         <v>24</v>
@@ -3146,7 +3146,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -3159,7 +3159,7 @@
         <v>41</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>19</v>
@@ -3174,31 +3174,31 @@
         <v>130</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H27" s="9">
         <v>25</v>
@@ -3207,7 +3207,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>19</v>
@@ -3218,7 +3218,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>19</v>
@@ -3227,37 +3227,37 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S27" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="T27" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="T27" s="12" t="s">
+      <c r="U27" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="U27" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H28" s="9">
         <v>26</v>
@@ -3266,7 +3266,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>19</v>
@@ -3277,7 +3277,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>19</v>
@@ -3286,37 +3286,37 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S28" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="T28" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="T28" s="12" t="s">
+      <c r="U28" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H29" s="9">
         <v>27</v>
@@ -3325,7 +3325,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3338,7 +3338,7 @@
         <v>121</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P29" s="9" t="s">
         <v>19</v>
@@ -3353,31 +3353,31 @@
         <v>130</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H30" s="9">
         <v>28</v>
@@ -3386,7 +3386,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3399,7 +3399,7 @@
         <v>51</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>20</v>
@@ -3414,29 +3414,29 @@
         <v>130</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H31" s="9">
         <v>29</v>
@@ -3445,7 +3445,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>19</v>
@@ -3456,7 +3456,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P31" s="9" t="s">
         <v>19</v>
@@ -3465,37 +3465,37 @@
         <v>7</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H32" s="9">
         <v>30</v>
@@ -3504,7 +3504,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3517,7 +3517,7 @@
         <v>33</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>19</v>
@@ -3532,31 +3532,31 @@
         <v>130</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H33" s="9">
         <v>31</v>
@@ -3565,7 +3565,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>20</v>
@@ -3578,7 +3578,7 @@
         <v>36</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>20</v>
@@ -3593,31 +3593,31 @@
         <v>130</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>123</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H34" s="9">
         <v>32</v>
@@ -3626,7 +3626,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3639,7 +3639,7 @@
         <v>121</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P34" s="9" t="s">
         <v>19</v>
@@ -3654,21 +3654,21 @@
         <v>130</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U34" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>124</v>
@@ -3676,7 +3676,7 @@
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H35" s="9">
         <v>33</v>
@@ -3685,7 +3685,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3698,7 +3698,7 @@
         <v>43</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P35" s="9" t="s">
         <v>19</v>
@@ -3713,21 +3713,21 @@
         <v>130</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>124</v>
@@ -3735,7 +3735,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="9"/>
       <c r="G36" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H36" s="9">
         <v>34</v>
@@ -3744,7 +3744,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3757,7 +3757,7 @@
         <v>24</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P36" s="9" t="s">
         <v>19</v>
@@ -3772,21 +3772,21 @@
         <v>130</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U36" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>124</v>
@@ -3794,7 +3794,7 @@
       <c r="E37" s="13"/>
       <c r="F37" s="9"/>
       <c r="G37" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H37" s="9">
         <v>35</v>
@@ -3803,7 +3803,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>20</v>
@@ -3816,7 +3816,7 @@
         <v>43</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P37" s="9" t="s">
         <v>19</v>
@@ -3831,21 +3831,21 @@
         <v>130</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U37" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>124</v>
@@ -3853,7 +3853,7 @@
       <c r="E38" s="13"/>
       <c r="F38" s="9"/>
       <c r="G38" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H38" s="9">
         <v>36</v>
@@ -3862,7 +3862,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>20</v>
@@ -3875,7 +3875,7 @@
         <v>120</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P38" s="9" t="s">
         <v>19</v>
@@ -3896,15 +3896,15 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>125</v>
@@ -3923,7 +3923,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>20</v>
@@ -3943,15 +3943,15 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>125</v>
@@ -3970,7 +3970,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>20</v>
@@ -3998,21 +3998,21 @@
         <v>130</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="U40" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>134</v>
+        <v>310</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>127</v>
@@ -4029,7 +4029,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>20</v>
@@ -4042,7 +4042,7 @@
         <v>52</v>
       </c>
       <c r="O41" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P41" s="9" t="s">
         <v>20</v>
@@ -4063,7 +4063,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
@@ -4086,7 +4086,7 @@
       <c r="T42" s="12"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
@@ -4109,7 +4109,7 @@
       <c r="T43" s="12"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
@@ -4132,7 +4132,7 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
@@ -4155,7 +4155,7 @@
       <c r="T45" s="12"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
@@ -4178,7 +4178,7 @@
       <c r="T46" s="12"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
@@ -4201,7 +4201,7 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
@@ -4224,7 +4224,7 @@
       <c r="T48" s="12"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
@@ -4247,7 +4247,7 @@
       <c r="T49" s="12"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
@@ -4270,7 +4270,7 @@
       <c r="T50" s="12"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
@@ -4293,7 +4293,7 @@
       <c r="T51" s="12"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
@@ -4316,7 +4316,7 @@
       <c r="T52" s="12"/>
       <c r="U52" s="10"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
@@ -4339,7 +4339,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
@@ -4362,7 +4362,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="10"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
@@ -4385,7 +4385,7 @@
       <c r="T55" s="12"/>
       <c r="U55" s="10"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
@@ -4408,7 +4408,7 @@
       <c r="T56" s="12"/>
       <c r="U56" s="10"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
@@ -4431,7 +4431,7 @@
       <c r="T57" s="12"/>
       <c r="U57" s="10"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
@@ -4454,7 +4454,7 @@
       <c r="T58" s="12"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -4477,7 +4477,7 @@
       <c r="T59" s="12"/>
       <c r="U59" s="10"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
@@ -4500,7 +4500,7 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
@@ -4523,7 +4523,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="10"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
@@ -4546,7 +4546,7 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
@@ -4569,7 +4569,7 @@
       <c r="T63" s="12"/>
       <c r="U63" s="10"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
@@ -4592,7 +4592,7 @@
       <c r="T64" s="12"/>
       <c r="U64" s="10"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
@@ -4615,7 +4615,7 @@
       <c r="T65" s="12"/>
       <c r="U65" s="10"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -4638,7 +4638,7 @@
       <c r="T66" s="12"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
@@ -4661,7 +4661,7 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A68" s="4"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
@@ -4684,7 +4684,7 @@
       <c r="T68" s="12"/>
       <c r="U68" s="10"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A69" s="4"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
@@ -4707,7 +4707,7 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A70" s="4"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
@@ -4730,7 +4730,7 @@
       <c r="T70" s="12"/>
       <c r="U70" s="10"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A71" s="4"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14"/>
@@ -4753,7 +4753,7 @@
       <c r="T71" s="12"/>
       <c r="U71" s="10"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A72" s="4"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -4776,7 +4776,7 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
-    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A73" s="4"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14"/>
@@ -4799,7 +4799,7 @@
       <c r="T73" s="12"/>
       <c r="U73" s="10"/>
     </row>
-    <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A74" s="4"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14"/>
@@ -4822,7 +4822,7 @@
       <c r="T74" s="12"/>
       <c r="U74" s="10"/>
     </row>
-    <row r="75" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A75" s="4"/>
       <c r="B75" s="13"/>
       <c r="C75" s="14"/>
@@ -4845,7 +4845,7 @@
       <c r="T75" s="12"/>
       <c r="U75" s="10"/>
     </row>
-    <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A76" s="4"/>
       <c r="B76" s="13"/>
       <c r="C76" s="14"/>
@@ -4868,7 +4868,7 @@
       <c r="T76" s="12"/>
       <c r="U76" s="10"/>
     </row>
-    <row r="77" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A77" s="4"/>
       <c r="B77" s="13"/>
       <c r="C77" s="14"/>
@@ -4891,7 +4891,7 @@
       <c r="T77" s="12"/>
       <c r="U77" s="10"/>
     </row>
-    <row r="78" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A78" s="4"/>
       <c r="B78" s="13"/>
       <c r="C78" s="14"/>
@@ -4914,378 +4914,372 @@
       <c r="T78" s="12"/>
       <c r="U78" s="10"/>
     </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="290" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="289" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="290" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="291" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="292" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5300,6 +5294,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5350,27 +5350,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="2"/>
-    <col min="14" max="14" width="24.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
+    <col min="13" max="13" width="11.3984375" style="2"/>
+    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -5411,7 +5411,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -5430,7 +5430,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -5449,7 +5449,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -5465,7 +5465,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -5514,7 +5514,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -5529,7 +5529,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -5544,7 +5544,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -5559,7 +5559,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -5574,7 +5574,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -5589,7 +5589,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -5604,7 +5604,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -5619,7 +5619,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -5634,7 +5634,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -5648,7 +5648,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -5662,7 +5662,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -5676,7 +5676,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -5690,7 +5690,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -5705,7 +5705,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -5720,7 +5720,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -5735,7 +5735,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -5750,7 +5750,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -5765,7 +5765,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -5780,7 +5780,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -5795,7 +5795,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -5810,7 +5810,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -5825,7 +5825,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -5840,7 +5840,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -5855,7 +5855,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -5870,7 +5870,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -5885,7 +5885,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -5900,7 +5900,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -5915,7 +5915,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -5930,7 +5930,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -5945,7 +5945,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -5960,7 +5960,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -5975,7 +5975,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5990,7 +5990,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -6005,7 +6005,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -6020,7 +6020,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -6035,7 +6035,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -6050,7 +6050,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -6065,7 +6065,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -6080,7 +6080,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -6095,7 +6095,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -6110,7 +6110,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -6122,7 +6122,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -6134,7 +6134,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -6147,7 +6147,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -6160,7 +6160,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -6173,7 +6173,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -6186,7 +6186,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -6199,7 +6199,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -6212,7 +6212,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -6225,7 +6225,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -6238,7 +6238,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -6251,7 +6251,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -6264,7 +6264,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -6277,7 +6277,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -6290,7 +6290,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -6303,7 +6303,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -6316,7 +6316,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -6329,7 +6329,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -6342,7 +6342,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -6355,7 +6355,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -6368,7 +6368,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -6381,7 +6381,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -6394,7 +6394,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -6408,7 +6408,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -6422,7 +6422,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -6436,7 +6436,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -6450,7 +6450,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -6464,7 +6464,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -6478,7 +6478,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -6492,7 +6492,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -6506,7 +6506,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -6520,7 +6520,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -6534,7 +6534,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -6548,7 +6548,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -6562,7 +6562,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -6576,7 +6576,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -6590,7 +6590,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -6604,7 +6604,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -6618,7 +6618,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -6632,7 +6632,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -6646,7 +6646,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -6660,7 +6660,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -6674,7 +6674,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -6688,7 +6688,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -6702,7 +6702,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -6716,7 +6716,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -6730,7 +6730,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -6744,7 +6744,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -6758,7 +6758,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -6772,7 +6772,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -6786,7 +6786,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -6800,7 +6800,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -6814,7 +6814,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -6828,7 +6828,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -6842,7 +6842,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -6856,7 +6856,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -6870,7 +6870,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -6884,7 +6884,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -6898,7 +6898,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -6912,7 +6912,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -6926,7 +6926,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -6940,7 +6940,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -6954,7 +6954,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -6968,7 +6968,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -6982,7 +6982,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6996,7 +6996,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -7010,7 +7010,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -7024,7 +7024,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -7038,7 +7038,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -7052,7 +7052,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -7066,7 +7066,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -7080,7 +7080,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -7094,7 +7094,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -7108,7 +7108,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -7122,7 +7122,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -7136,7 +7136,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -7150,7 +7150,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -7164,7 +7164,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -7178,7 +7178,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -7192,7 +7192,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -7206,7 +7206,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7220,7 +7220,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -7234,7 +7234,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -7248,7 +7248,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -7262,7 +7262,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>